<commit_message>
Update repo data based on source changes
</commit_message>
<xml_diff>
--- a/docs/data/citizens_assembly_register/0/citizens_assembly_register.xlsx
+++ b/docs/data/citizens_assembly_register/0/citizens_assembly_register.xlsx
@@ -33,8 +33,7 @@
     <t>Dataset description</t>
   </si>
   <si>
-    <t xml:space="preserve">Dataset of known citizen assemblies in the UK and their reports
-</t>
+    <t>Dataset of known citizen assemblies in the UK and their reports.  See the [GitHub page](https://github.com/mysociety/citizen-assembly-data#readme) for instructions on adding new data.</t>
   </si>
   <si>
     <t>Licence</t>
@@ -46,7 +45,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Contributors</t>
@@ -130,367 +129,421 @@
     <t>NHS</t>
   </si>
   <si>
+    <t>GLG</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>DUD</t>
+  </si>
+  <si>
+    <t>NWM</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>ADU</t>
+  </si>
+  <si>
+    <t>WND</t>
+  </si>
+  <si>
+    <t>BEN</t>
+  </si>
+  <si>
+    <t>LDS</t>
+  </si>
+  <si>
+    <t>NTCA</t>
+  </si>
+  <si>
+    <t>WSM</t>
+  </si>
+  <si>
     <t>LAC</t>
   </si>
   <si>
+    <t>BNE</t>
+  </si>
+  <si>
     <t>OXO</t>
   </si>
   <si>
-    <t>WSM</t>
+    <t>WAW</t>
+  </si>
+  <si>
+    <t>LBH</t>
   </si>
   <si>
     <t>STH</t>
   </si>
   <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>TES</t>
+  </si>
+  <si>
     <t>KTT</t>
   </si>
   <si>
-    <t>NWM</t>
-  </si>
-  <si>
-    <t>WND</t>
-  </si>
-  <si>
-    <t>GLG</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>ADU</t>
-  </si>
-  <si>
     <t>WFT</t>
   </si>
   <si>
-    <t>NTCA</t>
-  </si>
-  <si>
-    <t>BST</t>
-  </si>
-  <si>
-    <t>LDS</t>
-  </si>
-  <si>
     <t>HEF</t>
   </si>
   <si>
+    <t>WLV</t>
+  </si>
+  <si>
     <t>BGW</t>
   </si>
   <si>
-    <t>CMD</t>
-  </si>
-  <si>
-    <t>DUD</t>
-  </si>
-  <si>
-    <t>TES</t>
-  </si>
-  <si>
-    <t>BAR</t>
-  </si>
-  <si>
-    <t>BNE</t>
-  </si>
-  <si>
-    <t>LBH</t>
-  </si>
-  <si>
-    <t>WAW</t>
-  </si>
-  <si>
-    <t>WLV</t>
-  </si>
-  <si>
-    <t>BEN</t>
+    <t>Glasgow City Council</t>
+  </si>
+  <si>
+    <t>Barrow-in-Furness Borough Council</t>
+  </si>
+  <si>
+    <t>Copeland Borough Council</t>
+  </si>
+  <si>
+    <t>Dudley Metropolitan Borough Council</t>
+  </si>
+  <si>
+    <t>London Borough of Newham</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>University of Manchester and Information Commissioner’s Office</t>
+  </si>
+  <si>
+    <t>Devon County Council</t>
+  </si>
+  <si>
+    <t>Greater Cambridge Partnership</t>
+  </si>
+  <si>
+    <t>Adur District Council</t>
+  </si>
+  <si>
+    <t>London Borough of Wandsworth</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>London Borough of Brent</t>
+  </si>
+  <si>
+    <t>Leeds City Council</t>
+  </si>
+  <si>
+    <t>North of Tyne Combined Authority</t>
+  </si>
+  <si>
+    <t>City of Westminster</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Kendal Town Council</t>
   </si>
   <si>
     <t>Lancaster City Council</t>
   </si>
   <si>
-    <t>Jersey</t>
-  </si>
-  <si>
-    <t>UK</t>
+    <t>UCL</t>
+  </si>
+  <si>
+    <t>London Borough of Barnet</t>
   </si>
   <si>
     <t>Oxford City Council</t>
   </si>
   <si>
-    <t>City of Westminster</t>
-  </si>
-  <si>
-    <t>Scotland</t>
-  </si>
-  <si>
-    <t>University of Manchester and Information Commissioner’s Office</t>
+    <t>NHS Gloucestershire Clinical Commissioning Group</t>
+  </si>
+  <si>
+    <t>Warwick District Council</t>
+  </si>
+  <si>
+    <t>London Borough of Lambeth</t>
   </si>
   <si>
     <t>Southampton City Council</t>
   </si>
   <si>
+    <t>Bristol City Council</t>
+  </si>
+  <si>
+    <t>Brighton and Hove City Council</t>
+  </si>
+  <si>
+    <t>London Borough of Camden</t>
+  </si>
+  <si>
+    <t>Test Valley Borough Council</t>
+  </si>
+  <si>
     <t>Royal Borough of Kingston upon Thames</t>
   </si>
   <si>
-    <t>London Borough of Newham</t>
-  </si>
-  <si>
-    <t>London Borough of Wandsworth</t>
-  </si>
-  <si>
-    <t>Glasgow City Council</t>
-  </si>
-  <si>
-    <t>Copeland Borough Council</t>
-  </si>
-  <si>
-    <t>Devon County Council</t>
-  </si>
-  <si>
-    <t>Adur District Council</t>
-  </si>
-  <si>
     <t>London Borough of Waltham Forest</t>
   </si>
   <si>
-    <t>North of Tyne Combined Authority</t>
-  </si>
-  <si>
-    <t>Kendal Town Council</t>
-  </si>
-  <si>
-    <t>Brighton and Hove City Council</t>
-  </si>
-  <si>
-    <t>Leeds City Council</t>
-  </si>
-  <si>
     <t>Herefordshire Council</t>
   </si>
   <si>
+    <t>City of Wolverhampton Council</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
     <t>Blaenau Gwent County Borough Council</t>
   </si>
   <si>
-    <t>London Borough of Camden</t>
-  </si>
-  <si>
-    <t>Wales</t>
-  </si>
-  <si>
-    <t>UCL</t>
-  </si>
-  <si>
-    <t>Dudley Metropolitan Borough Council</t>
-  </si>
-  <si>
-    <t>Test Valley Borough Council</t>
-  </si>
-  <si>
-    <t>Barrow-in-Furness Borough Council</t>
-  </si>
-  <si>
-    <t>London Borough of Barnet</t>
-  </si>
-  <si>
-    <t>London Borough of Lambeth</t>
-  </si>
-  <si>
-    <t>Warwick District Council</t>
-  </si>
-  <si>
-    <t>City of Wolverhampton Council</t>
-  </si>
-  <si>
-    <t>London Borough of Brent</t>
-  </si>
-  <si>
-    <t>Greater Cambridge Partnership</t>
-  </si>
-  <si>
-    <t>Bristol City Council</t>
-  </si>
-  <si>
-    <t>NHS Gloucestershire Clinical Commissioning Group</t>
+    <t>https://barrowbc.gov.uk/climate-emergency/citizens-jury/</t>
+  </si>
+  <si>
+    <t>https://consultcambs.uk.engagementhq.com/greater-cambridge-citizens-assembly</t>
   </si>
   <si>
     <t>https://www.climateassembly.uk</t>
   </si>
   <si>
+    <t>https://engage.barnet.gov.uk/barnets-citizen-assembly</t>
+  </si>
+  <si>
+    <t>https://www.brighton-hove.gov.uk/environment/brighton-hove-climate-assembly-findings-report#tab--3-the-assemblys-recommendations</t>
+  </si>
+  <si>
     <t>https://sites.google.com/demsoc.org/newhamcitizensassembly-15-mins/greening-the-borough</t>
   </si>
   <si>
-    <t>https://www.brighton-hove.gov.uk/environment/brighton-hove-climate-assembly-findings-report#tab--3-the-assemblys-recommendations</t>
-  </si>
-  <si>
-    <t>https://barrowbc.gov.uk/climate-emergency/citizens-jury/</t>
-  </si>
-  <si>
-    <t>https://engage.barnet.gov.uk/barnets-citizen-assembly</t>
-  </si>
-  <si>
-    <t>https://consultcambs.uk.engagementhq.com/greater-cambridge-citizens-assembly</t>
+    <t>https://www.glasgow.gov.uk/CHttpHandler.ashx?id=55053&amp;p=0</t>
+  </si>
+  <si>
+    <t>https://sharedfuturecic.org.uk/wp-content/uploads/2022/03/Furness-Citizens-Jury-on-Climate-Change-Report-Final.pdf</t>
+  </si>
+  <si>
+    <t>https://sharedfuturecic.org.uk/wp-content/uploads/2021/11/Copeland-report-v0.4.pdf</t>
+  </si>
+  <si>
+    <t>https://www.dudley.gov.uk/media/13831/dudley-peoples-panel-report.pdf</t>
+  </si>
+  <si>
+    <t>https://www.newham.gov.uk/downloads/file/1885/newham-citizens-assembly-on-climate-change-final-report-2020</t>
+  </si>
+  <si>
+    <t>https://www.gov.je/SiteCollectionDocuments/Caring%20and%20support/ID%20Jersey%20Assisted%20Dying%20Citizens%27%20Jury%20Final%20Report%20FINAL.pdf</t>
+  </si>
+  <si>
+    <t>http://assets.mhs.manchester.ac.uk/gmpstrc/C4-AI-citizens-juries-report.pdf</t>
+  </si>
+  <si>
+    <t>https://devonclimateemergency.org.uk/wp-content/uploads/2021/10/FINAL-Devon-Climate-Assembly-Report-V10.pdf</t>
+  </si>
+  <si>
+    <t>https://www.involve.org.uk/sites/default/files/field/attachemnt/GCCA%20on%20Congestion%20Air%20Quality%20and%20Public%20Transport%20-%20Full%20Report%20.pdf</t>
+  </si>
+  <si>
+    <t>https://www.adur-worthing.gov.uk/media/Media,159369,smxx.pdf</t>
+  </si>
+  <si>
+    <t>https://wandsworth.gov.uk/media/13723/wandsworth_citizens_assembly_on_air_quality.pdf</t>
+  </si>
+  <si>
+    <t>https://www.climateassembly.uk/report/read/final-report.pdf</t>
+  </si>
+  <si>
+    <t>https://legacy.brent.gov.uk/media/16416373/climate_assembly_report2020.pdf</t>
+  </si>
+  <si>
+    <t>https://www.leedsclimate.org.uk/sites/default/files/REPORT%20V1.2%20FINAL.pdf</t>
+  </si>
+  <si>
+    <t>https://www.northoftyne-ca.gov.uk/wp-content/uploads/2021/07/NTCA-Citizens-Assembly-on-Climate-Change-report.pdf</t>
+  </si>
+  <si>
+    <t>https://www.westminster.gov.uk/tackling-climate-change-westminster/residents-communities-and-climate-action/climate-assembly</t>
+  </si>
+  <si>
+    <t>https://citizensassembly.theapsgroup.scot/report/files/assets/common/downloads/Citizens%20Assembly%20Main%20Report.pdf?uni=cf2dd1870a43fb4580bc43337ffe3142</t>
+  </si>
+  <si>
+    <t>https://www.kendalclimatejury.org/wp-content/uploads/2021/01/KendalClimateChangeJuryRecomendations.pdf</t>
   </si>
   <si>
     <t>https://www.lancaster.gov.uk/assets/attach/10184/People-s-Jury-report.pdf</t>
   </si>
   <si>
-    <t>https://www.gov.je/SiteCollectionDocuments/Caring%20and%20support/ID%20Jersey%20Assisted%20Dying%20Citizens%27%20Jury%20Final%20Report%20FINAL.pdf</t>
-  </si>
-  <si>
-    <t>https://www.climateassembly.uk/report/read/final-report.pdf</t>
+    <t>https://www.ucl.ac.uk/constitution-unit/sites/constitution_unit/files/report_2_final_digital.pdf</t>
+  </si>
+  <si>
+    <t>https://engage.barnet.gov.uk/25268/widgets/72520/documents/44063</t>
   </si>
   <si>
     <t>https://www.oxford.gov.uk/download/downloads/id/6871/oxford_citizens_assembly_on_climate_change_report_-_november_2019.pdf</t>
   </si>
   <si>
-    <t>https://www.westminster.gov.uk/tackling-climate-change-westminster/residents-communities-and-climate-action/climate-assembly</t>
+    <t>https://citizensjuries.org/wp-content/uploads/2020/02/Jurors-Report-1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.warwickdc.gov.uk/download/downloads/id/6687/the_district_of_warwick_people_s_inquiry_on_climate_change_202021.pdf</t>
+  </si>
+  <si>
+    <t>https://www.lambeth.gov.uk/sites/default/files/2021-08/Lambeth%20CA_Recommendations_Report.pdf</t>
+  </si>
+  <si>
+    <t>https://www.southampton.gov.uk/our-green-city/how-you-can-help/southampton-citizens-climate-assembly/</t>
+  </si>
+  <si>
+    <t>https://files.smartsurvey.io/2/0/T2H0LYNZ/BD13941__BCA_Report_V4_PRINT.pdf</t>
+  </si>
+  <si>
+    <t>https://www.camden.gov.uk/documents/20142/0/Camden+Citizens%27+Assembly+on+the+Climate+Crisis+-+Report.pdf/947eb4e5-5623-17a1-9964-46f351446548</t>
+  </si>
+  <si>
+    <t>https://www.camden.gov.uk/documents/20142/1006758/Camden+Health+and+Care+Citizens%27+Assembly+-+Final+Report+%28full%29.pdf/c7250d37-5c6c-5778-0c83-7105864a184c?t=1608110668706&amp;download=true</t>
   </si>
   <si>
     <t>https://web.archive.org/web/20211215142757/https://www.climateassembly.scot/sites/default/files/2021-09/620640_SCT0521502140-001_Scotland%E2%80%99s%20Climate%20Assembly_Final%20Report%20Goals_WEB%20ONLY%20VERSION.pdf</t>
   </si>
   <si>
-    <t>http://assets.mhs.manchester.ac.uk/gmpstrc/C4-AI-citizens-juries-report.pdf</t>
-  </si>
-  <si>
-    <t>https://www.southampton.gov.uk/our-green-city/how-you-can-help/southampton-citizens-climate-assembly/</t>
+    <t>https://www.demsoc.org/uploads/store/mediaupload/163/file/Romsey%20Citizens'%20Assembly%20Report%20December%202019.pdf</t>
   </si>
   <si>
     <t>https://www.kingston.gov.uk/downloads/file/419/kingston-citizens-assembly-on-air-quality-full-report-2020</t>
   </si>
   <si>
-    <t>https://www.newham.gov.uk/downloads/file/1885/newham-citizens-assembly-on-climate-change-final-report-2020</t>
-  </si>
-  <si>
-    <t>https://citizensassembly.theapsgroup.scot/report/files/assets/common/downloads/Citizens%20Assembly%20Main%20Report.pdf?uni=cf2dd1870a43fb4580bc43337ffe3142</t>
-  </si>
-  <si>
-    <t>https://wandsworth.gov.uk/media/13723/wandsworth_citizens_assembly_on_air_quality.pdf</t>
-  </si>
-  <si>
-    <t>https://www.glasgow.gov.uk/CHttpHandler.ashx?id=55053&amp;p=0</t>
-  </si>
-  <si>
-    <t>https://sharedfuturecic.org.uk/wp-content/uploads/2021/11/Copeland-report-v0.4.pdf</t>
-  </si>
-  <si>
-    <t>https://devonclimateemergency.org.uk/wp-content/uploads/2021/10/FINAL-Devon-Climate-Assembly-Report-V10.pdf</t>
-  </si>
-  <si>
-    <t>https://www.adur-worthing.gov.uk/media/Media,159369,smxx.pdf</t>
-  </si>
-  <si>
     <t>https://www.walthamforest.gov.uk/sites/default/files/2022-04/KD_WFCA_Recommendations_Report.pdf</t>
   </si>
   <si>
-    <t>https://www.northoftyne-ca.gov.uk/wp-content/uploads/2021/07/NTCA-Citizens-Assembly-on-Climate-Change-report.pdf</t>
-  </si>
-  <si>
-    <t>https://www.kendalclimatejury.org/wp-content/uploads/2021/01/KendalClimateChangeJuryRecomendations.pdf</t>
-  </si>
-  <si>
-    <t>https://www.leedsclimate.org.uk/sites/default/files/REPORT%20V1.2%20FINAL.pdf</t>
+    <t>https://citizensjuries.org/wp-content/uploads/2021/02/GLOS-CCG-FFTF-2021-CJ-Jurors-Report-v1.pdf</t>
+  </si>
+  <si>
+    <t>https://statesassembly.gov.je/assemblyreports/2021/r.95-2021.pdf</t>
   </si>
   <si>
     <t>https://councillors.herefordshire.gov.uk/documents/s50099605/Corrected%20Recommendations%20-%20Citizens%20Climate%20Assembly%20published.pdf</t>
   </si>
   <si>
+    <t>https://www.wolverhampton.gov.uk/sites/default/files/2020-09/Citizens%20Assembly%20Report.pdf</t>
+  </si>
+  <si>
+    <t>https://web.archive.org/web/20211118032534/https://static1.squarespace.com/static/5ca4d0b5fb18200e164e81b6/t/5d9c99a0209e7437725ecce9/1570544034964/citizen-assembly-English.pdf</t>
+  </si>
+  <si>
     <t>https://cynnalcymru.com/wp-content/uploads/2021/05/Blaenau-Gwent-Climate-Assembly-Report-ENG.pdf</t>
   </si>
   <si>
-    <t>https://www.camden.gov.uk/documents/20142/1006758/Camden+Health+and+Care+Citizens%27+Assembly+-+Final+Report+%28full%29.pdf/c7250d37-5c6c-5778-0c83-7105864a184c?t=1608110668706&amp;download=true</t>
-  </si>
-  <si>
-    <t>https://www.camden.gov.uk/documents/20142/0/Camden+Citizens%27+Assembly+on+the+Climate+Crisis+-+Report.pdf/947eb4e5-5623-17a1-9964-46f351446548</t>
-  </si>
-  <si>
-    <t>https://web.archive.org/web/20211118032534/https://static1.squarespace.com/static/5ca4d0b5fb18200e164e81b6/t/5d9c99a0209e7437725ecce9/1570544034964/citizen-assembly-English.pdf</t>
-  </si>
-  <si>
-    <t>https://www.ucl.ac.uk/constitution-unit/sites/constitution_unit/files/report_2_final_digital.pdf</t>
-  </si>
-  <si>
-    <t>https://www.dudley.gov.uk/media/13831/dudley-peoples-panel-report.pdf</t>
-  </si>
-  <si>
-    <t>https://www.demsoc.org/uploads/store/mediaupload/163/file/Romsey%20Citizens'%20Assembly%20Report%20December%202019.pdf</t>
-  </si>
-  <si>
-    <t>https://sharedfuturecic.org.uk/wp-content/uploads/2022/03/Furness-Citizens-Jury-on-Climate-Change-Report-Final.pdf</t>
-  </si>
-  <si>
-    <t>https://engage.barnet.gov.uk/25268/widgets/72520/documents/44063</t>
-  </si>
-  <si>
-    <t>https://www.lambeth.gov.uk/sites/default/files/2021-08/Lambeth%20CA_Recommendations_Report.pdf</t>
-  </si>
-  <si>
-    <t>https://www.warwickdc.gov.uk/download/downloads/id/6687/the_district_of_warwick_people_s_inquiry_on_climate_change_202021.pdf</t>
-  </si>
-  <si>
-    <t>https://www.wolverhampton.gov.uk/sites/default/files/2020-09/Citizens%20Assembly%20Report.pdf</t>
-  </si>
-  <si>
-    <t>https://legacy.brent.gov.uk/media/16416373/climate_assembly_report2020.pdf</t>
-  </si>
-  <si>
-    <t>https://www.involve.org.uk/sites/default/files/field/attachemnt/GCCA%20on%20Congestion%20Air%20Quality%20and%20Public%20Transport%20-%20Full%20Report%20.pdf</t>
-  </si>
-  <si>
-    <t>https://files.smartsurvey.io/2/0/T2H0LYNZ/BD13941__BCA_Report_V4_PRINT.pdf</t>
-  </si>
-  <si>
-    <t>https://citizensjuries.org/wp-content/uploads/2020/02/Jurors-Report-1.pdf</t>
-  </si>
-  <si>
-    <t>https://statesassembly.gov.je/assemblyreports/2021/r.95-2021.pdf</t>
-  </si>
-  <si>
-    <t>https://citizensjuries.org/wp-content/uploads/2021/02/GLOS-CCG-FFTF-2021-CJ-Jurors-Report-v1.pdf</t>
+    <t>Ipsos MORI</t>
+  </si>
+  <si>
+    <t>The Democratic Society</t>
+  </si>
+  <si>
+    <t>Involve</t>
   </si>
   <si>
     <t>Shared Future</t>
   </si>
   <si>
-    <t>Involve</t>
-  </si>
-  <si>
-    <t>Ipsos MORI</t>
+    <t>Traverse</t>
+  </si>
+  <si>
+    <t>Kaleidoscope Health &amp; Care</t>
   </si>
   <si>
     <t>Involve Foundation</t>
   </si>
   <si>
-    <t>The Democratic Society</t>
-  </si>
-  <si>
-    <t>Kaleidoscope Health &amp; Care</t>
+    <t>BritainThinks</t>
   </si>
   <si>
     <t>Sortition Foundation and Involve Foundation</t>
   </si>
   <si>
-    <t>Traverse</t>
-  </si>
-  <si>
-    <t>BritainThinks</t>
-  </si>
-  <si>
     <t>Finished</t>
   </si>
   <si>
     <t>Ongoing</t>
   </si>
   <si>
+    <t>Glasgow Citizens' Assembly on the Climate Emergency</t>
+  </si>
+  <si>
+    <t>The Furness Citizens’ Jury on Climate Change was a deliberative process that took place from November 2021 to February 2022. It was sponsored through funding from the National Lottery Climate Action Fund and Barrow Borough Council. The aim of the jury was to involve members of the local population in identifying ideas, strategies, and actions to address the climate emergency in the Furness area.</t>
+  </si>
+  <si>
+    <t>The Copeland People's Panel on Climate Change was a deliberative process that aimed to engage with citizens on how to address the challenge of the climate emergency. The panel consisted of 30 diverse members of the local population who came together over a period of two months to discuss and share their opinions on climate change and its impact on Copeland. The panel received presentations from experts and worked collaboratively to develop a set of 22 recommendations on addressing climate change in the region. The recommendations cover various topics such as transport, education, energy generation, and behavior change. The panel's work was sponsored through funding from the National Lottery Climate Action Fund and Copeland Borough Council.</t>
+  </si>
+  <si>
+    <t>Developing recommendations for making Dudley and Brierley Hill town centres vibrant and welcoming</t>
+  </si>
+  <si>
+    <t>The Newham Citizens’ Assembly on Climate Change brought together 36 randomly selected residents from the London Borough of Newham for three evenings and a weekend in February 2020 to develop recommendations in response to the question: “How can the council and residents work together to reach the aspiration of being carbon zero by 2050 at the latest?” Assembly members developed six themes to frame their recommendations to the Council.</t>
+  </si>
+  <si>
+    <t>A citizens' jury in Jersey was convened to consider the question of whether assisted dying should be permitted in the country, and if so, under what circumstances. The jury heard from a range of speakers, discussed the topic, and completed three different votes to provide a final response. The recommendations from the jury will inform a States Assembly debate on assisted dying.</t>
+  </si>
+  <si>
+    <t>A report of two citizens’ juries designed to explore whether automated decisions that affect people should require an explanation, even if that impacts AI performance</t>
+  </si>
+  <si>
+    <t>The Devon Climate Assembly brought together residents from across Devon to deliberate on key challenges in how Devon should respond to the climate emergency. The assembly focused on topics such as the role of onshore wind in the renewable energy strategy, encouraging less car use, and retrofitting homes and businesses to reduce carbon emissions. The assembly met for eleven sessions during June and July 2021 and was convened and facilitated by Involve, a public participation charity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greater Cambridge citizens assembly on congestion, air quality and public transport. </t>
+  </si>
+  <si>
+    <t>The Adur &amp; Worthing Climate Assembly was held in 2020 to discuss how to collectively tackle climate change and support the area to thrive. The assembly members, randomly selected from the Adur District and Worthing Borough, met virtually over five weekends to deliberate on the issue. The recommendations from the assembly cover various themes such as green spaces and biodiversity, information and education, green finance and energy, and planning.</t>
+  </si>
+  <si>
+    <t>The Wandsworth Citizens' Assembly on Air Quality was a deliberative process commissioned by Wandsworth Council to address the issue of air pollution in the borough. The assembly aimed to involve the public in identifying strategies and actions to improve air quality and address climate change. The assembly members, selected through a lottery process, spent four full Saturdays discussing, learning, and deliberating on the topic. They received presentations from commentators and had the opportunity to question them. The assembly produced a set of fifty recommendations on how to tackle air quality in Wandsworth, which will form the basis of a new Air Quality Action Plan.</t>
+  </si>
+  <si>
+    <t>The Climate Assembly UK was a unique process that brought together a diverse group of 108 citizens from all walks of life in the UK. The assembly aimed to discuss and prioritize actions that the UK should take to achieve net zero emissions by 2050. The assembly members engaged in discussions, debates, and voting to reach their recommendations. Their recommendations cover various areas, including transportation, energy use in homes, food and land usage, and consumer choices. The assembly emphasized the importance of education and information, fairness, freedom and choice, co-benefits, and the protection and restoration of the natural environment. They also highlighted the need for strong and clear leadership from the government, cross-party consensus, and long-term planning.</t>
+  </si>
+  <si>
+    <t>Recommendations from Assembly members to Brent Council on addressing climate change</t>
+  </si>
+  <si>
+    <t>The Leeds Climate Change Citizens' Jury was a deliberative process commissioned by the Leeds Climate Commission and designed and facilitated by the social enterprise Shared Future. It aimed to gather the opinions and recommendations of local residents on what Leeds should do about the climate emergency.</t>
+  </si>
+  <si>
+    <t>The North of Tyne Citizens' Assembly on Climate Change was commissioned by the North of Tyne Combined Authority (NTCA) to engage with citizens on how to address the challenge of the climate emergency. The Assembly consisted of 49 members who were chosen through a lottery to reflect the diversity of the local population. Over a period of five midweek evening sessions, a Saturday morning, and two full day Sunday sessions, the Assembly discussed, deliberated, and produced a set of 30 recommendations on how to address climate change in the region.</t>
+  </si>
+  <si>
+    <t>The Citizens’ Climate Assembly is being held to improve the representation of residents’ views in tackling the climate emergency.</t>
+  </si>
+  <si>
+    <t>Report of the Citizens' Assembly of Scotland</t>
+  </si>
+  <si>
+    <t>The Kendal Climate Change Citizen's Jury was held in the summer of 2020 and consisted of 20 Kendal residents who reflected the diversity of the community. Over four months, the jury listened to outside experts, considered relevant information, and worked together to come up with recommendations on what Kendal should do about the emergency of climate change.</t>
+  </si>
+  <si>
     <t>The Lancaster district Climate Change People’s Jury was a deliberative process commissioned by Lancaster City Council to address the climate emergency. It involved thirty residents from across the district who were recruited through a stratified sampling process. The jury met for sixteen sessions between February and October 2020 to discuss and answer the question of what needs to be done in homes, neighborhoods, and districts to respond to the emergency of climate change. The process included presentations from expert witnesses and deliberation among the jury members. The jury's goal was to reach a set of recommendations on how the Lancaster district can best address the climate emergency.</t>
   </si>
   <si>
-    <t>A citizens' jury in Jersey was convened to consider the question of whether assisted dying should be permitted in the country, and if so, under what circumstances. The jury heard from a range of speakers, discussed the topic, and completed three different votes to provide a final response. The recommendations from the jury will inform a States Assembly debate on assisted dying.</t>
-  </si>
-  <si>
-    <t>The Climate Assembly UK was a unique process that brought together a diverse group of 108 citizens from all walks of life in the UK. The assembly aimed to discuss and prioritize actions that the UK should take to achieve net zero emissions by 2050. The assembly members engaged in discussions, debates, and voting to reach their recommendations. Their recommendations cover various areas, including transportation, energy use in homes, food and land usage, and consumer choices. The assembly emphasized the importance of education and information, fairness, freedom and choice, co-benefits, and the protection and restoration of the natural environment. They also highlighted the need for strong and clear leadership from the government, cross-party consensus, and long-term planning.</t>
+    <t>Report of the Citizens' Assembly on Democracy in the UK</t>
+  </si>
+  <si>
+    <t>Barnet’s Citizens’ Assembly and Young People’s Assembly on Climate Change &amp; Biodiversity</t>
   </si>
   <si>
     <t xml:space="preserve">The Oxford Citizens Assembly on Climate Change was held in 2019. They
@@ -498,177 +551,123 @@
 </t>
   </si>
   <si>
-    <t>The Citizens’ Climate Assembly is being held to improve the representation of residents’ views in tackling the climate emergency.</t>
+    <t>This is a report from the 16 members of the citizens’ jury who met over five days to hear evidence and make recommendations about specialist hospital services in Gloucestershire.</t>
+  </si>
+  <si>
+    <t>People’s Inquiry on Climate Change. How can we in Adur and Worthing collectively tackle climate change and support our places to thrive?</t>
+  </si>
+  <si>
+    <t>Lambeth's Citizens' Assembly on Climate Change</t>
+  </si>
+  <si>
+    <t>Residents of Southampton are invited to participate in the shaping of the Citizens Assembly on climate change and transport. The council, along with the University of Southampton and public participation charity Involve, are seeking input from residents to help shape the approach and gather a broad range of perspectives. The Southampton Citizens’ Climate Assembly aims to deliver positive change in the city.</t>
+  </si>
+  <si>
+    <t>The Citizens’ Assembly was a group of 60 people broadly reflective of the population of Bristol, who came together over four weekends to consider how we recover from COVID-19 and create a better future for all in Bristol.</t>
+  </si>
+  <si>
+    <t>A citizens' assembly focused on reducing carbon emissions from transport and helping Brighton &amp; Hove become carbon neutral by 2030.</t>
+  </si>
+  <si>
+    <t>Newham's first permanent Citizens' Assembly in 2021, where 50 residents joined to identify creative ideas to make Newham’s green spaces better and more accessible.</t>
+  </si>
+  <si>
+    <t>The Camden Citizens’ Assembly on the Climate Crisis brought together over 50 randomly selected residents from Camden during July 2019 to develop an approach for how Camden can best tackle the climate crisis.</t>
+  </si>
+  <si>
+    <t>The Health and Care Citizens’ Assembly in Camden was held in 2020 to gather the voice of residents and shape the common purpose of the integrated care partnership and inform Camden’s new Joint Health and Wellbeing Strategy. The assembly focused on addressing health inequalities, ensuring health services meet individual needs, and improving communication between services and residents. The assembly process involved face-to-face and online events, and members were encouraged to share their experiences and expectations to guide future change to the health and care system.</t>
   </si>
   <si>
     <t>Scotland's Climate Assembly is Scotland's first citizens' assembly focused on climate change. It brought together over 100 ordinary citizens from across Scotland to deliberate about the climate emergency and make recommendations for action.</t>
   </si>
   <si>
-    <t>A report of two citizens’ juries designed to explore whether automated decisions that affect people should require an explanation, even if that impacts AI performance</t>
-  </si>
-  <si>
-    <t>Residents of Southampton are invited to participate in the shaping of the Citizens Assembly on climate change and transport. The council, along with the University of Southampton and public participation charity Involve, are seeking input from residents to help shape the approach and gather a broad range of perspectives. The Southampton Citizens’ Climate Assembly aims to deliver positive change in the city.</t>
+    <t>Developing recommendations for improving the area around Crosfield Hall and the Bus Station in Romsey</t>
   </si>
   <si>
     <t>The RBK Citizens’ Assembly on Air Quality brought together 38 randomly selected residents from the Royal Borough of Kingston upon Thames for two weekends during November and December 2019 to develop recommendations on how to collectively improve air quality in the borough.</t>
   </si>
   <si>
-    <t>The Newham Citizens’ Assembly on Climate Change brought together 36 randomly selected residents from the London Borough of Newham for three evenings and a weekend in February 2020 to develop recommendations in response to the question: “How can the council and residents work together to reach the aspiration of being carbon zero by 2050 at the latest?” Assembly members developed six themes to frame their recommendations to the Council.</t>
-  </si>
-  <si>
-    <t>Report of the Citizens' Assembly of Scotland</t>
-  </si>
-  <si>
-    <t>The Wandsworth Citizens' Assembly on Air Quality was a deliberative process commissioned by Wandsworth Council to address the issue of air pollution in the borough. The assembly aimed to involve the public in identifying strategies and actions to improve air quality and address climate change. The assembly members, selected through a lottery process, spent four full Saturdays discussing, learning, and deliberating on the topic. They received presentations from commentators and had the opportunity to question them. The assembly produced a set of fifty recommendations on how to tackle air quality in Wandsworth, which will form the basis of a new Air Quality Action Plan.</t>
-  </si>
-  <si>
-    <t>Glasgow Citizens' Assembly on the Climate Emergency</t>
-  </si>
-  <si>
-    <t>Newham's first permanent Citizens' Assembly in 2021, where 50 residents joined to identify creative ideas to make Newham’s green spaces better and more accessible.</t>
-  </si>
-  <si>
-    <t>The Copeland People's Panel on Climate Change was a deliberative process that aimed to engage with citizens on how to address the challenge of the climate emergency. The panel consisted of 30 diverse members of the local population who came together over a period of two months to discuss and share their opinions on climate change and its impact on Copeland. The panel received presentations from experts and worked collaboratively to develop a set of 22 recommendations on addressing climate change in the region. The recommendations cover various topics such as transport, education, energy generation, and behavior change. The panel's work was sponsored through funding from the National Lottery Climate Action Fund and Copeland Borough Council.</t>
-  </si>
-  <si>
-    <t>The Devon Climate Assembly brought together residents from across Devon to deliberate on key challenges in how Devon should respond to the climate emergency. The assembly focused on topics such as the role of onshore wind in the renewable energy strategy, encouraging less car use, and retrofitting homes and businesses to reduce carbon emissions. The assembly met for eleven sessions during June and July 2021 and was convened and facilitated by Involve, a public participation charity.</t>
-  </si>
-  <si>
-    <t>The Adur &amp; Worthing Climate Assembly was held in 2020 to discuss how to collectively tackle climate change and support the area to thrive. The assembly members, randomly selected from the Adur District and Worthing Borough, met virtually over five weekends to deliberate on the issue. The recommendations from the assembly cover various themes such as green spaces and biodiversity, information and education, green finance and energy, and planning.</t>
-  </si>
-  <si>
     <t>The Waltham Forest Citizens Assembly was a group of 34 individuals who came together over three weekends to consider how to stop hate crime and make the borough equally welcoming and safe.</t>
   </si>
   <si>
-    <t>The North of Tyne Citizens' Assembly on Climate Change was commissioned by the North of Tyne Combined Authority (NTCA) to engage with citizens on how to address the challenge of the climate emergency. The Assembly consisted of 49 members who were chosen through a lottery to reflect the diversity of the local population. Over a period of five midweek evening sessions, a Saturday morning, and two full day Sunday sessions, the Assembly discussed, deliberated, and produced a set of 30 recommendations on how to address climate change in the region.</t>
-  </si>
-  <si>
-    <t>The Kendal Climate Change Citizen's Jury was held in the summer of 2020 and consisted of 20 Kendal residents who reflected the diversity of the community. Over four months, the jury listened to outside experts, considered relevant information, and worked together to come up with recommendations on what Kendal should do about the emergency of climate change.</t>
-  </si>
-  <si>
-    <t>A citizens' assembly focused on reducing carbon emissions from transport and helping Brighton &amp; Hove become carbon neutral by 2030.</t>
-  </si>
-  <si>
-    <t>The Leeds Climate Change Citizens' Jury was a deliberative process commissioned by the Leeds Climate Commission and designed and facilitated by the social enterprise Shared Future. It aimed to gather the opinions and recommendations of local residents on what Leeds should do about the climate emergency.</t>
+    <t>Assessment of the 2020 Fit for the Future public consultation process and information, and recommendations about the outcomes.</t>
+  </si>
+  <si>
+    <t>Report of Jersey's Citizens' Assembly on Climate Change</t>
   </si>
   <si>
     <t>Herefordshire Council held a Citizens' Climate Assembly to address the challenges of Climate Change. The assembly aimed to engage residents in the democratic process, have open and honest dialogue, and achieve consensus on actions needed in the county.</t>
   </si>
   <si>
+    <t>Mini citizens’ assembly on climate change</t>
+  </si>
+  <si>
+    <t>This citizens assembly aims to address the issue of climate change and develop strategies for reducing greenhouse gas emissions.</t>
+  </si>
+  <si>
     <t>The Blaenau Gwent Climate Assembly was held to address the question of what should be done in Blaenau Gwent to tackle the climate crisis in a fair and sustainable way. Assembly members met for 23 hours, heard from over 20 experts, and produced recommendations on topics such as housing retrofit, transport, and green space.</t>
   </si>
   <si>
-    <t>The Health and Care Citizens’ Assembly in Camden was held in 2020 to gather the voice of residents and shape the common purpose of the integrated care partnership and inform Camden’s new Joint Health and Wellbeing Strategy. The assembly focused on addressing health inequalities, ensuring health services meet individual needs, and improving communication between services and residents. The assembly process involved face-to-face and online events, and members were encouraged to share their experiences and expectations to guide future change to the health and care system.</t>
-  </si>
-  <si>
-    <t>The Camden Citizens’ Assembly on the Climate Crisis brought together over 50 randomly selected residents from Camden during July 2019 to develop an approach for how Camden can best tackle the climate crisis.</t>
-  </si>
-  <si>
-    <t>This citizens assembly aims to address the issue of climate change and develop strategies for reducing greenhouse gas emissions.</t>
-  </si>
-  <si>
-    <t>Report of the Citizens' Assembly on Democracy in the UK</t>
-  </si>
-  <si>
-    <t>Developing recommendations for making Dudley and Brierley Hill town centres vibrant and welcoming</t>
-  </si>
-  <si>
-    <t>Developing recommendations for improving the area around Crosfield Hall and the Bus Station in Romsey</t>
-  </si>
-  <si>
-    <t>The Furness Citizens’ Jury on Climate Change was a deliberative process that took place from November 2021 to February 2022. It was sponsored through funding from the National Lottery Climate Action Fund and Barrow Borough Council. The aim of the jury was to involve members of the local population in identifying ideas, strategies, and actions to address the climate emergency in the Furness area.</t>
-  </si>
-  <si>
-    <t>Barnet’s Citizens’ Assembly and Young People’s Assembly on Climate Change &amp; Biodiversity</t>
-  </si>
-  <si>
-    <t>Lambeth's Citizens' Assembly on Climate Change</t>
-  </si>
-  <si>
-    <t>People’s Inquiry on Climate Change. How can we in Adur and Worthing collectively tackle climate change and support our places to thrive?</t>
-  </si>
-  <si>
-    <t>Mini citizens’ assembly on climate change</t>
-  </si>
-  <si>
-    <t>Recommendations from Assembly members to Brent Council on addressing climate change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greater Cambridge citizens assembly on congestion, air quality and public transport. </t>
-  </si>
-  <si>
-    <t>The Citizens’ Assembly was a group of 60 people broadly reflective of the population of Bristol, who came together over four weekends to consider how we recover from COVID-19 and create a better future for all in Bristol.</t>
-  </si>
-  <si>
-    <t>This is a report from the 16 members of the citizens’ jury who met over five days to hear evidence and make recommendations about specialist hospital services in Gloucestershire.</t>
-  </si>
-  <si>
-    <t>Report of Jersey's Citizens' Assembly on Climate Change</t>
-  </si>
-  <si>
-    <t>Assessment of the 2020 Fit for the Future public consultation process and information, and recommendations about the outcomes.</t>
-  </si>
-  <si>
     <t>Climate Assembly</t>
   </si>
   <si>
+    <t>Climate Change</t>
+  </si>
+  <si>
+    <t>Town centre revitalization</t>
+  </si>
+  <si>
     <t>Assisted Dying</t>
   </si>
   <si>
     <t>AI Explainability</t>
   </si>
   <si>
+    <t>Transport/Environment</t>
+  </si>
+  <si>
     <t>Air Quality</t>
   </si>
   <si>
     <t>Political Reform</t>
   </si>
   <si>
+    <t>Democracy UK</t>
+  </si>
+  <si>
+    <t>Specialist hospital</t>
+  </si>
+  <si>
+    <t>COVID-19 Recovery</t>
+  </si>
+  <si>
     <t>Greening the Borough</t>
   </si>
   <si>
-    <t>Climate Change</t>
+    <t>Health and Care</t>
+  </si>
+  <si>
+    <t>Vision for Romsey</t>
   </si>
   <si>
     <t>Hate crime</t>
   </si>
   <si>
-    <t>Health and Care</t>
-  </si>
-  <si>
-    <t>Democracy UK</t>
-  </si>
-  <si>
-    <t>Town centre revitalization</t>
-  </si>
-  <si>
-    <t>Vision for Romsey</t>
-  </si>
-  <si>
-    <t>Transport/Environment</t>
-  </si>
-  <si>
-    <t>COVID-19 Recovery</t>
-  </si>
-  <si>
-    <t>Specialist hospital</t>
-  </si>
-  <si>
     <t>Fit for the Future</t>
   </si>
   <si>
+    <t># this was hard to track down - scotlands two domains don't work anymnore</t>
+  </si>
+  <si>
+    <t>no pdf version, example of report spread over multiple pages</t>
+  </si>
+  <si>
+    <t>not clearly avalaible anywhere</t>
+  </si>
+  <si>
     <t>does this have to be rehosted to be scraped?</t>
   </si>
   <si>
-    <t># this was hard to track down - scotlands two domains don't work anymnore</t>
-  </si>
-  <si>
-    <t>not clearly avalaible anywhere</t>
-  </si>
-  <si>
-    <t>no pdf version, example of report spread over multiple pages</t>
-  </si>
-  <si>
     <t>not linked at all on website</t>
   </si>
   <si>
@@ -678,246 +677,246 @@
     <t>mySocietySearch</t>
   </si>
   <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-glg-2021-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bar-2022-climate-change.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cop-2021-climate-change.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-dud-2019-town-centre-revitalization.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-nwm-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-jersey-2021-assisted-dying.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-university-of-manchester-and-information-commissioners-office-2019-ai-explainability.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-dev-2021-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-greater-cambridge-partnership-2023-transport-environment.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-adu-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wnd-2023-air-quality.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-uk-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-ben-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-lds-2019-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-ntca-2021-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wsm-2023-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-scotland-2021-political-reform.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-kendal-town-council-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-lac-2020-climate-assembly.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-jersey-2021-assisted-dying.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-uk-2020-climate-assembly.pdf</t>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-ucl-2021-democracy-uk.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bne-2023-climate-change.pdf</t>
   </si>
   <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-oxo-2019-climate-assembly.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wsm-2023-climate-assembly.pdf</t>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-nhs-gloucestershire-clinical-commissioning-group-2020-specialist-hospital.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-waw-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-lbh-2021-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-sth-2023-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bst-2021-covid-19-recovery.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cmd-2019-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cmd-2020-health-and-care.pdf</t>
   </si>
   <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-scotland-2021-climate-assembly.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-university-of-manchester-and-information-commissioners-office-2019-ai-explainability.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-sth-2023-climate-assembly.pdf</t>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-tes-2019-vision-for-romsey.pdf</t>
   </si>
   <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-ktt-2020-air-quality.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-nwm-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-scotland-2021-political-reform.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wnd-2023-air-quality.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-glg-2021-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cop-2021-climate-change.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-dev-2021-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-adu-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wft-2020-hate-crime.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-ntca-2021-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-kendal-town-council-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-lds-2019-climate-assembly.pdf</t>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-nhs-gloucestershire-clinical-commissioning-group-2021-fit-for-the-future.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-jersey-2021-climate-assembly.pdf</t>
   </si>
   <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-hef-2022-climate-assembly.pdf</t>
   </si>
   <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wlv-2020-climate-assembly.pdf</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-wales-2022-climate-assembly.pdf</t>
+  </si>
+  <si>
     <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bgw-2021-climate-assembly.pdf</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cmd-2020-health-and-care.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-cmd-2019-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/n-wales-2022-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-ucl-2021-democracy-uk.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-dud-2019-town-centre-revitalization.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-tes-2019-vision-for-romsey.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bar-2022-climate-change.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bne-2023-climate-change.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-lbh-2021-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-waw-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-wlv-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-ben-2020-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-greater-cambridge-partnership-2023-transport-environment.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/la-bst-2021-covid-19-recovery.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-nhs-gloucestershire-clinical-commissioning-group-2020-specialist-hospital.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-jersey-2021-climate-assembly.pdf</t>
-  </si>
-  <si>
-    <t>https://raw.githubusercontent.com/mysociety/citizen-assembly-data/main//data/raw/reports/org-nhs-gloucestershire-clinical-commissioning-group-2021-fit-for-the-future.pdf</t>
+    <t>la-glg-2021-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-bar-2022-climate-change</t>
+  </si>
+  <si>
+    <t>la-cop-2021-climate-change</t>
+  </si>
+  <si>
+    <t>la-dud-2019-town-centre-revitalization</t>
+  </si>
+  <si>
+    <t>la-nwm-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>org-jersey-2021-assisted-dying</t>
+  </si>
+  <si>
+    <t>org-university-of-manchester-and-information-commissioners-office-2019-ai-explainability</t>
+  </si>
+  <si>
+    <t>la-dev-2021-climate-assembly</t>
+  </si>
+  <si>
+    <t>org-greater-cambridge-partnership-2023-transport-environment</t>
+  </si>
+  <si>
+    <t>la-adu-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-wnd-2023-air-quality</t>
+  </si>
+  <si>
+    <t>n-uk-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-ben-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-lds-2019-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-ntca-2021-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-wsm-2023-climate-assembly</t>
+  </si>
+  <si>
+    <t>n-scotland-2021-political-reform</t>
+  </si>
+  <si>
+    <t>org-kendal-town-council-2020-climate-assembly</t>
   </si>
   <si>
     <t>la-lac-2020-climate-assembly</t>
   </si>
   <si>
-    <t>org-jersey-2021-assisted-dying</t>
-  </si>
-  <si>
-    <t>n-uk-2020-climate-assembly</t>
+    <t>org-ucl-2021-democracy-uk</t>
+  </si>
+  <si>
+    <t>la-bne-2023-climate-change</t>
   </si>
   <si>
     <t>la-oxo-2019-climate-assembly</t>
   </si>
   <si>
-    <t>la-wsm-2023-climate-assembly</t>
+    <t>org-nhs-gloucestershire-clinical-commissioning-group-2020-specialist-hospital</t>
+  </si>
+  <si>
+    <t>la-waw-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-lbh-2021-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-sth-2023-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-bst-2021-covid-19-recovery</t>
+  </si>
+  <si>
+    <t>la-bst-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-nwm-2021-greening-the-borough</t>
+  </si>
+  <si>
+    <t>la-cmd-2019-climate-assembly</t>
+  </si>
+  <si>
+    <t>la-cmd-2020-health-and-care</t>
   </si>
   <si>
     <t>n-scotland-2021-climate-assembly</t>
   </si>
   <si>
-    <t>org-university-of-manchester-and-information-commissioners-office-2019-ai-explainability</t>
-  </si>
-  <si>
-    <t>la-sth-2023-climate-assembly</t>
+    <t>la-tes-2019-vision-for-romsey</t>
   </si>
   <si>
     <t>la-ktt-2020-air-quality</t>
   </si>
   <si>
-    <t>la-nwm-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>n-scotland-2021-political-reform</t>
-  </si>
-  <si>
-    <t>la-wnd-2023-air-quality</t>
-  </si>
-  <si>
-    <t>la-glg-2021-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-nwm-2021-greening-the-borough</t>
-  </si>
-  <si>
-    <t>la-cop-2021-climate-change</t>
-  </si>
-  <si>
-    <t>la-dev-2021-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-adu-2020-climate-assembly</t>
-  </si>
-  <si>
     <t>la-wft-2020-hate-crime</t>
   </si>
   <si>
-    <t>la-ntca-2021-climate-assembly</t>
-  </si>
-  <si>
-    <t>org-kendal-town-council-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-bst-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-lds-2019-climate-assembly</t>
+    <t>org-nhs-gloucestershire-clinical-commissioning-group-2021-fit-for-the-future</t>
+  </si>
+  <si>
+    <t>org-jersey-2021-climate-assembly</t>
   </si>
   <si>
     <t>la-hef-2022-climate-assembly</t>
   </si>
   <si>
+    <t>la-wlv-2020-climate-assembly</t>
+  </si>
+  <si>
+    <t>n-wales-2022-climate-assembly</t>
+  </si>
+  <si>
     <t>la-bgw-2021-climate-assembly</t>
   </si>
   <si>
-    <t>la-cmd-2020-health-and-care</t>
-  </si>
-  <si>
-    <t>la-cmd-2019-climate-assembly</t>
-  </si>
-  <si>
-    <t>n-wales-2022-climate-assembly</t>
-  </si>
-  <si>
-    <t>org-ucl-2021-democracy-uk</t>
-  </si>
-  <si>
-    <t>la-dud-2019-town-centre-revitalization</t>
-  </si>
-  <si>
-    <t>la-tes-2019-vision-for-romsey</t>
-  </si>
-  <si>
-    <t>la-bar-2022-climate-change</t>
-  </si>
-  <si>
-    <t>la-bne-2023-climate-change</t>
-  </si>
-  <si>
-    <t>la-lbh-2021-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-waw-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-wlv-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>la-ben-2020-climate-assembly</t>
-  </si>
-  <si>
-    <t>org-greater-cambridge-partnership-2023-transport-environment</t>
-  </si>
-  <si>
-    <t>la-bst-2021-covid-19-recovery</t>
-  </si>
-  <si>
-    <t>org-nhs-gloucestershire-clinical-commissioning-group-2020-specialist-hospital</t>
-  </si>
-  <si>
-    <t>org-jersey-2021-climate-assembly</t>
-  </si>
-  <si>
-    <t>org-nhs-gloucestershire-clinical-commissioning-group-2021-fit-for-the-future</t>
-  </si>
-  <si>
     <t>column</t>
   </si>
   <si>
@@ -1002,7 +1001,7 @@
     <t>Finished, Ongoing</t>
   </si>
   <si>
-    <t>2020, 2021, 2019, 2023, 2022</t>
+    <t>2021, 2022, 2019, 2020, 2023</t>
   </si>
   <si>
     <t>InvolveTracker2021, mySocietySearch</t>
@@ -1569,10 +1568,10 @@
         <v>153</v>
       </c>
       <c r="H2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>155</v>
@@ -1592,25 +1591,28 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F3" t="s">
-        <v>145</v>
-      </c>
       <c r="G3" t="s">
         <v>153</v>
       </c>
       <c r="H3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="I3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>156</v>
@@ -1619,7 +1621,7 @@
         <v>197</v>
       </c>
       <c r="M3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>220</v>
@@ -1630,14 +1632,14 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>107</v>
       </c>
@@ -1645,16 +1647,16 @@
         <v>153</v>
       </c>
       <c r="H4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I4">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>157</v>
       </c>
       <c r="K4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="M4" t="s">
         <v>217</v>
@@ -1671,7 +1673,7 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>66</v>
@@ -1680,7 +1682,7 @@
         <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" t="s">
         <v>153</v>
@@ -1689,13 +1691,13 @@
         <v>2019</v>
       </c>
       <c r="I5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>158</v>
       </c>
       <c r="K5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M5" t="s">
         <v>217</v>
@@ -1712,7 +1714,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>67</v>
@@ -1721,13 +1723,13 @@
         <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H6">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="I6">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>159</v>
@@ -1736,7 +1738,7 @@
         <v>196</v>
       </c>
       <c r="M6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>223</v>
@@ -1747,7 +1749,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>68</v>
@@ -1755,6 +1757,9 @@
       <c r="E7" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="F7" t="s">
+        <v>146</v>
+      </c>
       <c r="G7" t="s">
         <v>153</v>
       </c>
@@ -1762,16 +1767,13 @@
         <v>2021</v>
       </c>
       <c r="I7">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>160</v>
       </c>
       <c r="K7" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="M7" t="s">
         <v>217</v>
@@ -1806,7 +1808,7 @@
         <v>161</v>
       </c>
       <c r="K8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M8" t="s">
         <v>217</v>
@@ -1823,7 +1825,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>70</v>
@@ -1832,10 +1834,13 @@
         <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9">
-        <v>2023</v>
+        <v>2021</v>
+      </c>
+      <c r="I9">
+        <v>70</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>162</v>
@@ -1844,7 +1849,7 @@
         <v>196</v>
       </c>
       <c r="M9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>226</v>
@@ -1855,34 +1860,34 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
         <v>153</v>
       </c>
       <c r="H10">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="I10">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>163</v>
       </c>
       <c r="K10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M10" t="s">
         <v>217</v>
@@ -1899,7 +1904,7 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>72</v>
@@ -1907,6 +1912,9 @@
       <c r="E11" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="F11" t="s">
+        <v>145</v>
+      </c>
       <c r="G11" t="s">
         <v>153</v>
       </c>
@@ -1914,7 +1922,7 @@
         <v>2020</v>
       </c>
       <c r="I11">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>164</v>
@@ -1934,34 +1942,37 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>115</v>
       </c>
+      <c r="F12" t="s">
+        <v>147</v>
+      </c>
       <c r="G12" t="s">
         <v>153</v>
       </c>
       <c r="H12">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="I12">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>165</v>
       </c>
       <c r="K12" t="s">
-        <v>200</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="M12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>229</v>
@@ -1972,37 +1983,34 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F13" t="s">
-        <v>144</v>
-      </c>
       <c r="G13" t="s">
         <v>153</v>
       </c>
       <c r="H13">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="I13">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>166</v>
       </c>
       <c r="K13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>230</v>
@@ -2016,25 +2024,22 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F14" t="s">
-        <v>146</v>
-      </c>
       <c r="G14" t="s">
         <v>153</v>
       </c>
       <c r="H14">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="I14">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>167</v>
@@ -2057,34 +2062,34 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="G15" t="s">
         <v>153</v>
       </c>
       <c r="H15">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="I15">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>168</v>
       </c>
       <c r="K15" t="s">
-        <v>201</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="M15" t="s">
         <v>217</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>271</v>
@@ -2095,13 +2100,13 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G16" t="s">
         <v>153</v>
@@ -2110,19 +2115,19 @@
         <v>2021</v>
       </c>
       <c r="I16">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>169</v>
       </c>
       <c r="K16" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="M16" t="s">
         <v>217</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>272</v>
@@ -2133,22 +2138,22 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H17">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="I17">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>170</v>
@@ -2157,10 +2162,10 @@
         <v>196</v>
       </c>
       <c r="M17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>273</v>
@@ -2168,40 +2173,37 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="G18" t="s">
         <v>153</v>
       </c>
       <c r="H18">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I18">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>196</v>
+        <v>203</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="M18" t="s">
         <v>217</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>274</v>
@@ -2209,19 +2211,13 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F19" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="G19" t="s">
         <v>153</v>
@@ -2230,19 +2226,19 @@
         <v>2020</v>
       </c>
       <c r="I19">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>172</v>
       </c>
       <c r="K19" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="M19" t="s">
         <v>217</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>275</v>
@@ -2256,19 +2252,22 @@
         <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="F20" t="s">
+        <v>147</v>
       </c>
       <c r="G20" t="s">
         <v>153</v>
       </c>
       <c r="H20">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="I20">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>173</v>
@@ -2280,7 +2279,7 @@
         <v>217</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>276</v>
@@ -2291,31 +2290,31 @@
         <v>34</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" t="s">
         <v>153</v>
       </c>
       <c r="H21">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>174</v>
       </c>
       <c r="K21" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="M21" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>277</v>
@@ -2329,34 +2328,34 @@
         <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" t="s">
-        <v>146</v>
+        <v>102</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="G22" t="s">
         <v>153</v>
       </c>
       <c r="H22">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="I22">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>175</v>
       </c>
       <c r="K22" t="s">
-        <v>196</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="M22" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>278</v>
@@ -2370,10 +2369,13 @@
         <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>144</v>
       </c>
       <c r="G23" t="s">
         <v>153</v>
@@ -2382,7 +2384,7 @@
         <v>2019</v>
       </c>
       <c r="I23">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>176</v>
@@ -2394,7 +2396,7 @@
         <v>217</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>279</v>
@@ -2402,37 +2404,34 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G24" t="s">
         <v>153</v>
       </c>
       <c r="H24">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="I24">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>177</v>
       </c>
       <c r="K24" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="M24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>280</v>
@@ -2443,22 +2442,25 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>147</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
       </c>
       <c r="H25">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="I25">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>178</v>
@@ -2466,14 +2468,11 @@
       <c r="K25" t="s">
         <v>196</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="M25" t="s">
         <v>217</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>281</v>
@@ -2484,37 +2483,37 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G26" t="s">
         <v>153</v>
       </c>
       <c r="H26">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I26">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>179</v>
       </c>
       <c r="K26" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="M26" t="s">
         <v>217</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>282</v>
@@ -2528,19 +2527,16 @@
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H27">
-        <v>2019</v>
-      </c>
-      <c r="I27">
-        <v>50</v>
+        <v>2023</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>180</v>
@@ -2549,10 +2545,10 @@
         <v>196</v>
       </c>
       <c r="M27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>283</v>
@@ -2560,37 +2556,37 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H28">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="I28">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>181</v>
       </c>
       <c r="K28" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="M28" t="s">
         <v>217</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>284</v>
@@ -2598,34 +2594,40 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>130</v>
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
+        <v>144</v>
       </c>
       <c r="G29" t="s">
         <v>153</v>
       </c>
       <c r="H29">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="I29">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>182</v>
       </c>
       <c r="K29" t="s">
-        <v>205</v>
+        <v>196</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="M29" t="s">
-        <v>218</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>285</v>
@@ -2636,37 +2638,34 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" t="s">
-        <v>148</v>
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="G30" t="s">
         <v>153</v>
       </c>
       <c r="H30">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="I30">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>183</v>
       </c>
       <c r="K30" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="M30" t="s">
         <v>217</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>286</v>
@@ -2680,7 +2679,7 @@
         <v>56</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>132</v>
@@ -2692,13 +2691,13 @@
         <v>2019</v>
       </c>
       <c r="I31">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>184</v>
       </c>
       <c r="K31" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="M31" t="s">
         <v>217</v>
@@ -2715,34 +2714,34 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="F32" t="s">
+        <v>149</v>
+      </c>
       <c r="G32" t="s">
         <v>153</v>
       </c>
       <c r="H32">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="I32">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>185</v>
       </c>
       <c r="K32" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="M32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>247</v>
@@ -2753,16 +2752,10 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>134</v>
@@ -2771,19 +2764,22 @@
         <v>153</v>
       </c>
       <c r="H33">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="I33">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>186</v>
       </c>
       <c r="K33" t="s">
-        <v>202</v>
+        <v>196</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="M33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>248</v>
@@ -2797,7 +2793,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>92</v>
@@ -2805,23 +2801,20 @@
       <c r="E34" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F34" t="s">
-        <v>151</v>
-      </c>
       <c r="G34" t="s">
         <v>153</v>
       </c>
       <c r="H34">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="I34">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>187</v>
       </c>
       <c r="K34" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="M34" t="s">
         <v>217</v>
@@ -2838,7 +2831,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>93</v>
@@ -2847,7 +2840,7 @@
         <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G35" t="s">
         <v>153</v>
@@ -2856,13 +2849,13 @@
         <v>2020</v>
       </c>
       <c r="I35">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>188</v>
       </c>
       <c r="K35" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="M35" t="s">
         <v>217</v>
@@ -2879,7 +2872,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>94</v>
@@ -2888,7 +2881,7 @@
         <v>137</v>
       </c>
       <c r="F36" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="G36" t="s">
         <v>153</v>
@@ -2897,16 +2890,16 @@
         <v>2020</v>
       </c>
       <c r="I36">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>189</v>
       </c>
       <c r="K36" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="M36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>251</v>
@@ -2917,13 +2910,10 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>138</v>
@@ -2932,16 +2922,16 @@
         <v>153</v>
       </c>
       <c r="H37">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I37">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>190</v>
       </c>
       <c r="K37" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="M37" t="s">
         <v>217</v>
@@ -2958,31 +2948,25 @@
         <v>34</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F38" t="s">
-        <v>145</v>
-      </c>
       <c r="G38" t="s">
         <v>153</v>
       </c>
       <c r="H38">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="I38">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>191</v>
       </c>
       <c r="K38" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="M38" t="s">
         <v>217</v>
@@ -2999,10 +2983,10 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>140</v>
@@ -3011,19 +2995,19 @@
         <v>153</v>
       </c>
       <c r="H39">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="I39">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>192</v>
       </c>
       <c r="K39" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="M39" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>254</v>
@@ -3034,14 +3018,20 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="F40" t="s">
+        <v>151</v>
+      </c>
       <c r="G40" t="s">
         <v>153</v>
       </c>
@@ -3055,10 +3045,10 @@
         <v>193</v>
       </c>
       <c r="K40" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="M40" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>255</v>
@@ -3069,22 +3059,25 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
       <c r="G41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H41">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="I41">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>194</v>
@@ -3104,7 +3097,10 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>98</v>
@@ -3119,13 +3115,16 @@
         <v>2021</v>
       </c>
       <c r="I42">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>195</v>
       </c>
       <c r="K42" t="s">
-        <v>211</v>
+        <v>196</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="M42" t="s">
         <v>217</v>
@@ -3141,9 +3140,9 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="N2" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="N3" r:id="rId4"/>
-    <hyperlink ref="D4" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="N3" r:id="rId5"/>
     <hyperlink ref="E4" r:id="rId6"/>
     <hyperlink ref="N4" r:id="rId7"/>
     <hyperlink ref="E5" r:id="rId8"/>
@@ -3156,63 +3155,63 @@
     <hyperlink ref="N8" r:id="rId15"/>
     <hyperlink ref="E9" r:id="rId16"/>
     <hyperlink ref="N9" r:id="rId17"/>
-    <hyperlink ref="E10" r:id="rId18"/>
-    <hyperlink ref="N10" r:id="rId19"/>
-    <hyperlink ref="E11" r:id="rId20"/>
-    <hyperlink ref="N11" r:id="rId21"/>
-    <hyperlink ref="E12" r:id="rId22"/>
-    <hyperlink ref="N12" r:id="rId23"/>
-    <hyperlink ref="E13" r:id="rId24"/>
-    <hyperlink ref="N13" r:id="rId25"/>
-    <hyperlink ref="E14" r:id="rId26"/>
-    <hyperlink ref="N14" r:id="rId27"/>
-    <hyperlink ref="D15" r:id="rId28"/>
-    <hyperlink ref="E16" r:id="rId29"/>
-    <hyperlink ref="N16" r:id="rId30"/>
-    <hyperlink ref="E17" r:id="rId31"/>
-    <hyperlink ref="N17" r:id="rId32"/>
-    <hyperlink ref="E18" r:id="rId33"/>
-    <hyperlink ref="N18" r:id="rId34"/>
-    <hyperlink ref="E19" r:id="rId35"/>
-    <hyperlink ref="N19" r:id="rId36"/>
-    <hyperlink ref="E20" r:id="rId37"/>
-    <hyperlink ref="N20" r:id="rId38"/>
-    <hyperlink ref="E21" r:id="rId39"/>
-    <hyperlink ref="N21" r:id="rId40"/>
-    <hyperlink ref="D22" r:id="rId41" location="tab--3-the-assemblys-recommendations"/>
-    <hyperlink ref="E23" r:id="rId42"/>
-    <hyperlink ref="N23" r:id="rId43"/>
-    <hyperlink ref="E24" r:id="rId44"/>
-    <hyperlink ref="N24" r:id="rId45"/>
-    <hyperlink ref="E25" r:id="rId46"/>
-    <hyperlink ref="N25" r:id="rId47"/>
-    <hyperlink ref="E26" r:id="rId48"/>
-    <hyperlink ref="N26" r:id="rId49"/>
-    <hyperlink ref="E27" r:id="rId50"/>
-    <hyperlink ref="N27" r:id="rId51"/>
-    <hyperlink ref="E28" r:id="rId52"/>
-    <hyperlink ref="N28" r:id="rId53"/>
-    <hyperlink ref="E29" r:id="rId54"/>
-    <hyperlink ref="N29" r:id="rId55"/>
-    <hyperlink ref="E30" r:id="rId56"/>
-    <hyperlink ref="N30" r:id="rId57"/>
-    <hyperlink ref="E31" r:id="rId58"/>
-    <hyperlink ref="N31" r:id="rId59"/>
-    <hyperlink ref="D32" r:id="rId60"/>
-    <hyperlink ref="E32" r:id="rId61"/>
-    <hyperlink ref="N32" r:id="rId62"/>
-    <hyperlink ref="D33" r:id="rId63"/>
-    <hyperlink ref="E33" r:id="rId64"/>
-    <hyperlink ref="N33" r:id="rId65"/>
-    <hyperlink ref="E34" r:id="rId66"/>
-    <hyperlink ref="N34" r:id="rId67"/>
-    <hyperlink ref="E35" r:id="rId68"/>
-    <hyperlink ref="N35" r:id="rId69"/>
-    <hyperlink ref="E36" r:id="rId70"/>
-    <hyperlink ref="N36" r:id="rId71"/>
-    <hyperlink ref="E37" r:id="rId72"/>
-    <hyperlink ref="N37" r:id="rId73"/>
-    <hyperlink ref="D38" r:id="rId74"/>
+    <hyperlink ref="D10" r:id="rId18"/>
+    <hyperlink ref="E10" r:id="rId19"/>
+    <hyperlink ref="N10" r:id="rId20"/>
+    <hyperlink ref="E11" r:id="rId21"/>
+    <hyperlink ref="N11" r:id="rId22"/>
+    <hyperlink ref="E12" r:id="rId23"/>
+    <hyperlink ref="N12" r:id="rId24"/>
+    <hyperlink ref="D13" r:id="rId25"/>
+    <hyperlink ref="E13" r:id="rId26"/>
+    <hyperlink ref="N13" r:id="rId27"/>
+    <hyperlink ref="E14" r:id="rId28"/>
+    <hyperlink ref="N14" r:id="rId29"/>
+    <hyperlink ref="E15" r:id="rId30"/>
+    <hyperlink ref="N15" r:id="rId31"/>
+    <hyperlink ref="E16" r:id="rId32"/>
+    <hyperlink ref="N16" r:id="rId33"/>
+    <hyperlink ref="E17" r:id="rId34"/>
+    <hyperlink ref="N17" r:id="rId35"/>
+    <hyperlink ref="E18" r:id="rId36"/>
+    <hyperlink ref="N18" r:id="rId37"/>
+    <hyperlink ref="E19" r:id="rId38"/>
+    <hyperlink ref="N19" r:id="rId39"/>
+    <hyperlink ref="E20" r:id="rId40"/>
+    <hyperlink ref="N20" r:id="rId41"/>
+    <hyperlink ref="E21" r:id="rId42"/>
+    <hyperlink ref="N21" r:id="rId43"/>
+    <hyperlink ref="D22" r:id="rId44"/>
+    <hyperlink ref="E22" r:id="rId45"/>
+    <hyperlink ref="N22" r:id="rId46"/>
+    <hyperlink ref="E23" r:id="rId47"/>
+    <hyperlink ref="N23" r:id="rId48"/>
+    <hyperlink ref="E24" r:id="rId49"/>
+    <hyperlink ref="N24" r:id="rId50"/>
+    <hyperlink ref="E25" r:id="rId51"/>
+    <hyperlink ref="N25" r:id="rId52"/>
+    <hyperlink ref="E26" r:id="rId53"/>
+    <hyperlink ref="N26" r:id="rId54"/>
+    <hyperlink ref="E27" r:id="rId55"/>
+    <hyperlink ref="N27" r:id="rId56"/>
+    <hyperlink ref="E28" r:id="rId57"/>
+    <hyperlink ref="N28" r:id="rId58"/>
+    <hyperlink ref="D29" r:id="rId59" location="tab--3-the-assemblys-recommendations"/>
+    <hyperlink ref="D30" r:id="rId60"/>
+    <hyperlink ref="E31" r:id="rId61"/>
+    <hyperlink ref="N31" r:id="rId62"/>
+    <hyperlink ref="E32" r:id="rId63"/>
+    <hyperlink ref="N32" r:id="rId64"/>
+    <hyperlink ref="E33" r:id="rId65"/>
+    <hyperlink ref="N33" r:id="rId66"/>
+    <hyperlink ref="E34" r:id="rId67"/>
+    <hyperlink ref="N34" r:id="rId68"/>
+    <hyperlink ref="E35" r:id="rId69"/>
+    <hyperlink ref="N35" r:id="rId70"/>
+    <hyperlink ref="E36" r:id="rId71"/>
+    <hyperlink ref="N36" r:id="rId72"/>
+    <hyperlink ref="E37" r:id="rId73"/>
+    <hyperlink ref="N37" r:id="rId74"/>
     <hyperlink ref="E38" r:id="rId75"/>
     <hyperlink ref="N38" r:id="rId76"/>
     <hyperlink ref="E39" r:id="rId77"/>
@@ -3295,7 +3294,7 @@
         <v>320</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>323</v>
@@ -3312,7 +3311,7 @@
         <v>320</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
         <v>323</v>
@@ -3329,7 +3328,7 @@
         <v>320</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
         <v>323</v>
@@ -3363,7 +3362,7 @@
         <v>320</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" t="s">
         <v>323</v>
@@ -3437,7 +3436,7 @@
         <v>320</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="E11" t="s">
         <v>324</v>
@@ -3454,7 +3453,7 @@
         <v>320</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
         <v>323</v>
@@ -3471,7 +3470,7 @@
         <v>320</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
         <v>323</v>
@@ -3508,7 +3507,7 @@
         <v>320</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E15" t="s">
         <v>323</v>
@@ -3525,7 +3524,7 @@
         <v>320</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E16" t="s">
         <v>324</v>

</xml_diff>